<commit_message>
Trying to creat split barplots
</commit_message>
<xml_diff>
--- a/MetaData.xlsx
+++ b/MetaData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="38">
   <si>
     <t>Code</t>
   </si>
@@ -570,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F255"/>
+  <dimension ref="A1:F256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H147" sqref="H147"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2835,7 +2835,7 @@
         <v>305</v>
       </c>
       <c r="C113" s="18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D113" s="4">
         <v>0</v>
@@ -3475,7 +3475,7 @@
         <v>369</v>
       </c>
       <c r="C145" s="18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D145" s="4">
         <v>48</v>
@@ -5569,10 +5569,10 @@
     </row>
     <row r="250" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A250">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B250">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C250" s="4">
         <v>10</v>
@@ -5584,15 +5584,15 @@
         <v>33</v>
       </c>
       <c r="F250" s="11">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="251" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A251">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B251">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C251" s="4">
         <v>10</v>
@@ -5604,15 +5604,15 @@
         <v>33</v>
       </c>
       <c r="F251" s="11">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="252" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A252">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B252">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C252" s="4">
         <v>10</v>
@@ -5621,18 +5621,18 @@
         <v>48</v>
       </c>
       <c r="E252" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F252" s="11">
-        <v>5.0000000000000001E-3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="253" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A253">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B253">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C253" s="4">
         <v>10</v>
@@ -5643,16 +5643,16 @@
       <c r="E253" t="s">
         <v>34</v>
       </c>
-      <c r="F253">
-        <v>0.05</v>
+      <c r="F253" s="11">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="254" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A254">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B254">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C254" s="4">
         <v>10</v>
@@ -5664,26 +5664,46 @@
         <v>34</v>
       </c>
       <c r="F254">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="255" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A255">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B255">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C255" s="4">
         <v>10</v>
       </c>
-      <c r="D255" s="16">
-        <v>48</v>
-      </c>
-      <c r="E255" s="13" t="s">
+      <c r="D255" s="4">
+        <v>48</v>
+      </c>
+      <c r="E255" t="s">
+        <v>34</v>
+      </c>
+      <c r="F255">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>528</v>
+      </c>
+      <c r="B256">
+        <v>528</v>
+      </c>
+      <c r="C256" s="4">
+        <v>10</v>
+      </c>
+      <c r="D256" s="16">
+        <v>48</v>
+      </c>
+      <c r="E256" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F255" s="13">
+      <c r="F256" s="13">
         <v>0</v>
       </c>
     </row>

</xml_diff>